<commit_message>
var03 is complete 16 - wrong answer
</commit_message>
<xml_diff>
--- a/var03/18.xlsx
+++ b/var03/18.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74706B48-9738-4399-AA24-38D39CC9B02D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="3615" yWindow="2685" windowWidth="28110" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,7 +138,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -258,6 +255,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -293,6 +307,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -468,19 +499,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AO42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AO23" sqref="AO23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="6.6328125" customWidth="1"/>
+    <col min="1" max="20" width="6.5703125" customWidth="1"/>
+    <col min="22" max="41" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
         <v>37</v>
       </c>
@@ -542,7 +574,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>49</v>
       </c>
@@ -604,7 +636,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>54</v>
       </c>
@@ -666,7 +698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>45</v>
       </c>
@@ -728,7 +760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>20</v>
       </c>
@@ -790,7 +822,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>25</v>
       </c>
@@ -852,7 +884,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>22</v>
       </c>
@@ -914,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>17</v>
       </c>
@@ -976,7 +1008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>55</v>
       </c>
@@ -1038,7 +1070,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>47</v>
       </c>
@@ -1100,7 +1132,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>17</v>
       </c>
@@ -1162,7 +1194,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>2</v>
       </c>
@@ -1224,7 +1256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>42</v>
       </c>
@@ -1286,7 +1318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>15</v>
       </c>
@@ -1348,7 +1380,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>57</v>
       </c>
@@ -1410,7 +1442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>40</v>
       </c>
@@ -1472,7 +1504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>18</v>
       </c>
@@ -1534,7 +1566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>37</v>
       </c>
@@ -1596,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>17</v>
       </c>
@@ -1658,7 +1690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>54</v>
       </c>
@@ -1718,6 +1750,3246 @@
       </c>
       <c r="T20" s="1">
         <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <f t="shared" ref="A23:A40" si="0">A24+A1 * MOD(A1 + 1,2)</f>
+        <v>252</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" ref="B23:B40" si="1">MAX(A23,B24) + B1 * MOD(B1 + 1,2)</f>
+        <v>252</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:C40" si="2">MAX(B23,C24) + C1 * MOD(C1 + 1,2)</f>
+        <v>452</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" ref="D23:D40" si="3">MAX(C23,D24) + D1 * MOD(D1 + 1,2)</f>
+        <v>628</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" ref="E23:E40" si="4">MAX(D23,E24) + E1 * MOD(E1 + 1,2)</f>
+        <v>690</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" ref="F23:F40" si="5">MAX(E23,F24) + F1 * MOD(F1 + 1,2)</f>
+        <v>724</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" ref="G23:G40" si="6">MAX(F23,G24) + G1 * MOD(G1 + 1,2)</f>
+        <v>734</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" ref="H23:H40" si="7">MAX(G23,H24) + H1 * MOD(H1 + 1,2)</f>
+        <v>772</v>
+      </c>
+      <c r="I23" s="4">
+        <f t="shared" ref="I23:I40" si="8">MAX(H23,I24) + I1 * MOD(I1 + 1,2)</f>
+        <v>810</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" ref="J23:J40" si="9">MAX(I23,J24) + J1 * MOD(J1 + 1,2)</f>
+        <v>810</v>
+      </c>
+      <c r="K23" s="4">
+        <f t="shared" ref="K23:K40" si="10">MAX(J23,K24) + K1 * MOD(K1 + 1,2)</f>
+        <v>846</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" ref="L23:L40" si="11">MAX(K23,L24) + L1 * MOD(L1 + 1,2)</f>
+        <v>874</v>
+      </c>
+      <c r="M23" s="4">
+        <f t="shared" ref="M23:M40" si="12">MAX(L23,M24) + M1 * MOD(M1 + 1,2)</f>
+        <v>916</v>
+      </c>
+      <c r="N23" s="4">
+        <f t="shared" ref="N23:N40" si="13">MAX(M23,N24) + N1 * MOD(N1 + 1,2)</f>
+        <v>916</v>
+      </c>
+      <c r="O23" s="4">
+        <f t="shared" ref="O23:O40" si="14">MAX(N23,O24) + O1 * MOD(O1 + 1,2)</f>
+        <v>964</v>
+      </c>
+      <c r="P23" s="4">
+        <f t="shared" ref="P23:P40" si="15">MAX(O23,P24) + P1 * MOD(P1 + 1,2)</f>
+        <v>964</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" ref="Q23:Q40" si="16">MAX(P23,Q24) + Q1 * MOD(Q1 + 1,2)</f>
+        <v>994</v>
+      </c>
+      <c r="R23" s="4">
+        <f t="shared" ref="R23:R40" si="17">MAX(Q23,R24) + R1 * MOD(R1 + 1,2)</f>
+        <v>994</v>
+      </c>
+      <c r="S23" s="4">
+        <f t="shared" ref="S23:S40" si="18">MAX(R23,S24) + S1 * MOD(S1 + 1,2)</f>
+        <v>1040</v>
+      </c>
+      <c r="T23" s="5">
+        <f t="shared" ref="T23:T40" si="19">MAX(S23,T24) + T1 * MOD(T1 + 1,2)</f>
+        <v>1102</v>
+      </c>
+      <c r="V23" s="3">
+        <f t="shared" ref="V23:V40" si="20">V24+A1 * MOD(A1 + 1,2)</f>
+        <v>252</v>
+      </c>
+      <c r="W23" s="4">
+        <f t="shared" ref="W23:W40" si="21">MIN(V23,W24) + B1 * MOD(B1 + 1,2)</f>
+        <v>166</v>
+      </c>
+      <c r="X23" s="4">
+        <f t="shared" ref="X23:X40" si="22">MIN(W23,X24) + C1 * MOD(C1 + 1,2)</f>
+        <v>166</v>
+      </c>
+      <c r="Y23" s="4">
+        <f t="shared" ref="Y23:Y40" si="23">MIN(X23,Y24) + D1 * MOD(D1 + 1,2)</f>
+        <v>172</v>
+      </c>
+      <c r="Z23" s="4">
+        <f t="shared" ref="Z23:Z40" si="24">MIN(Y23,Z24) + E1 * MOD(E1 + 1,2)</f>
+        <v>224</v>
+      </c>
+      <c r="AA23" s="4">
+        <f t="shared" ref="AA23:AA40" si="25">MIN(Z23,AA24) + F1 * MOD(F1 + 1,2)</f>
+        <v>218</v>
+      </c>
+      <c r="AB23" s="4">
+        <f t="shared" ref="AB23:AB40" si="26">MIN(AA23,AB24) + G1 * MOD(G1 + 1,2)</f>
+        <v>184</v>
+      </c>
+      <c r="AC23" s="4">
+        <f t="shared" ref="AC23:AC40" si="27">MIN(AB23,AC24) + H1 * MOD(H1 + 1,2)</f>
+        <v>184</v>
+      </c>
+      <c r="AD23" s="4">
+        <f t="shared" ref="AD23:AD40" si="28">MIN(AC23,AD24) + I1 * MOD(I1 + 1,2)</f>
+        <v>184</v>
+      </c>
+      <c r="AE23" s="4">
+        <f t="shared" ref="AE23:AE40" si="29">MIN(AD23,AE24) + J1 * MOD(J1 + 1,2)</f>
+        <v>184</v>
+      </c>
+      <c r="AF23" s="4">
+        <f t="shared" ref="AF23:AF40" si="30">MIN(AE23,AF24) + K1 * MOD(K1 + 1,2)</f>
+        <v>220</v>
+      </c>
+      <c r="AG23" s="4">
+        <f t="shared" ref="AG23:AG40" si="31">MIN(AF23,AG24) + L1 * MOD(L1 + 1,2)</f>
+        <v>202</v>
+      </c>
+      <c r="AH23" s="4">
+        <f t="shared" ref="AH23:AH40" si="32">MIN(AG23,AH24) + M1 * MOD(M1 + 1,2)</f>
+        <v>228</v>
+      </c>
+      <c r="AI23" s="4">
+        <f t="shared" ref="AI23:AI40" si="33">MIN(AH23,AI24) + N1 * MOD(N1 + 1,2)</f>
+        <v>218</v>
+      </c>
+      <c r="AJ23" s="4">
+        <f t="shared" ref="AJ23:AJ40" si="34">MIN(AI23,AJ24) + O1 * MOD(O1 + 1,2)</f>
+        <v>242</v>
+      </c>
+      <c r="AK23" s="4">
+        <f t="shared" ref="AK23:AK40" si="35">MIN(AJ23,AK24) + P1 * MOD(P1 + 1,2)</f>
+        <v>194</v>
+      </c>
+      <c r="AL23" s="4">
+        <f t="shared" ref="AL23:AL40" si="36">MIN(AK23,AL24) + Q1 * MOD(Q1 + 1,2)</f>
+        <v>202</v>
+      </c>
+      <c r="AM23" s="4">
+        <f t="shared" ref="AM23:AM40" si="37">MIN(AL23,AM24) + R1 * MOD(R1 + 1,2)</f>
+        <v>202</v>
+      </c>
+      <c r="AN23" s="4">
+        <f t="shared" ref="AN23:AN40" si="38">MIN(AM23,AN24) + S1 * MOD(S1 + 1,2)</f>
+        <v>234</v>
+      </c>
+      <c r="AO23" s="5">
+        <f t="shared" ref="AO23:AO40" si="39">MIN(AN23,AO24) + T1 * MOD(T1 + 1,2)</f>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="2"/>
+        <v>452</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="3"/>
+        <v>622</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="4"/>
+        <v>632</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="5"/>
+        <v>676</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="6"/>
+        <v>734</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="7"/>
+        <v>772</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="8"/>
+        <v>810</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="9"/>
+        <v>810</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="10"/>
+        <v>810</v>
+      </c>
+      <c r="L24" s="2">
+        <f t="shared" si="11"/>
+        <v>874</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="12"/>
+        <v>890</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="13"/>
+        <v>902</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="14"/>
+        <v>902</v>
+      </c>
+      <c r="P24" s="2">
+        <f t="shared" si="15"/>
+        <v>902</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="16"/>
+        <v>986</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="17"/>
+        <v>992</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="18"/>
+        <v>1008</v>
+      </c>
+      <c r="T24" s="7">
+        <f t="shared" si="19"/>
+        <v>1058</v>
+      </c>
+      <c r="V24" s="6">
+        <f t="shared" si="20"/>
+        <v>252</v>
+      </c>
+      <c r="W24" s="2">
+        <f t="shared" si="21"/>
+        <v>166</v>
+      </c>
+      <c r="X24" s="2">
+        <f t="shared" si="22"/>
+        <v>166</v>
+      </c>
+      <c r="Y24" s="2">
+        <f t="shared" si="23"/>
+        <v>166</v>
+      </c>
+      <c r="Z24" s="2">
+        <f t="shared" si="24"/>
+        <v>166</v>
+      </c>
+      <c r="AA24" s="2">
+        <f t="shared" si="25"/>
+        <v>184</v>
+      </c>
+      <c r="AB24" s="2">
+        <f t="shared" si="26"/>
+        <v>184</v>
+      </c>
+      <c r="AC24" s="2">
+        <f t="shared" si="27"/>
+        <v>184</v>
+      </c>
+      <c r="AD24" s="2">
+        <f t="shared" si="28"/>
+        <v>190</v>
+      </c>
+      <c r="AE24" s="2">
+        <f t="shared" si="29"/>
+        <v>190</v>
+      </c>
+      <c r="AF24" s="2">
+        <f t="shared" si="30"/>
+        <v>190</v>
+      </c>
+      <c r="AG24" s="2">
+        <f t="shared" si="31"/>
+        <v>202</v>
+      </c>
+      <c r="AH24" s="2">
+        <f t="shared" si="32"/>
+        <v>218</v>
+      </c>
+      <c r="AI24" s="2">
+        <f t="shared" si="33"/>
+        <v>218</v>
+      </c>
+      <c r="AJ24" s="2">
+        <f t="shared" si="34"/>
+        <v>194</v>
+      </c>
+      <c r="AK24" s="2">
+        <f t="shared" si="35"/>
+        <v>194</v>
+      </c>
+      <c r="AL24" s="2">
+        <f t="shared" si="36"/>
+        <v>234</v>
+      </c>
+      <c r="AM24" s="2">
+        <f t="shared" si="37"/>
+        <v>240</v>
+      </c>
+      <c r="AN24" s="2">
+        <f t="shared" si="38"/>
+        <v>240</v>
+      </c>
+      <c r="AO24" s="7">
+        <f t="shared" si="39"/>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <f t="shared" si="0"/>
+        <v>252</v>
+      </c>
+      <c r="B25" s="2">
+        <f t="shared" si="1"/>
+        <v>252</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="2"/>
+        <v>452</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="3"/>
+        <v>622</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="4"/>
+        <v>632</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" ref="F25:F30" si="40">F26 + F3 * MOD(F3 + 1,2)</f>
+        <v>658</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="6"/>
+        <v>734</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="7"/>
+        <v>772</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="8"/>
+        <v>804</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="9"/>
+        <v>804</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="10"/>
+        <v>806</v>
+      </c>
+      <c r="L25" s="2">
+        <f t="shared" si="11"/>
+        <v>862</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="12"/>
+        <v>870</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="13"/>
+        <v>902</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="14"/>
+        <v>902</v>
+      </c>
+      <c r="P25" s="2">
+        <f t="shared" si="15"/>
+        <v>902</v>
+      </c>
+      <c r="Q25" s="2">
+        <f t="shared" si="16"/>
+        <v>946</v>
+      </c>
+      <c r="R25" s="2">
+        <f t="shared" si="17"/>
+        <v>946</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="18"/>
+        <v>1008</v>
+      </c>
+      <c r="T25" s="7">
+        <f t="shared" si="19"/>
+        <v>1008</v>
+      </c>
+      <c r="V25" s="6">
+        <f t="shared" si="20"/>
+        <v>252</v>
+      </c>
+      <c r="W25" s="2">
+        <f t="shared" si="21"/>
+        <v>166</v>
+      </c>
+      <c r="X25" s="2">
+        <f t="shared" si="22"/>
+        <v>166</v>
+      </c>
+      <c r="Y25" s="2">
+        <f t="shared" si="23"/>
+        <v>206</v>
+      </c>
+      <c r="Z25" s="7">
+        <f t="shared" si="24"/>
+        <v>186</v>
+      </c>
+      <c r="AA25" s="2">
+        <f t="shared" ref="AA25:AA30" si="41">AA26 + F3 * MOD(F3 + 1,2)</f>
+        <v>200</v>
+      </c>
+      <c r="AB25" s="2">
+        <f t="shared" si="26"/>
+        <v>222</v>
+      </c>
+      <c r="AC25" s="2">
+        <f t="shared" si="27"/>
+        <v>202</v>
+      </c>
+      <c r="AD25" s="2">
+        <f t="shared" si="28"/>
+        <v>196</v>
+      </c>
+      <c r="AE25" s="2">
+        <f t="shared" si="29"/>
+        <v>196</v>
+      </c>
+      <c r="AF25" s="2">
+        <f t="shared" si="30"/>
+        <v>192</v>
+      </c>
+      <c r="AG25" s="2">
+        <f t="shared" si="31"/>
+        <v>248</v>
+      </c>
+      <c r="AH25" s="2">
+        <f t="shared" si="32"/>
+        <v>202</v>
+      </c>
+      <c r="AI25" s="2">
+        <f t="shared" si="33"/>
+        <v>226</v>
+      </c>
+      <c r="AJ25" s="2">
+        <f t="shared" si="34"/>
+        <v>194</v>
+      </c>
+      <c r="AK25" s="2">
+        <f t="shared" si="35"/>
+        <v>194</v>
+      </c>
+      <c r="AL25" s="2">
+        <f t="shared" si="36"/>
+        <v>238</v>
+      </c>
+      <c r="AM25" s="2">
+        <f t="shared" si="37"/>
+        <v>238</v>
+      </c>
+      <c r="AN25" s="2">
+        <f t="shared" si="38"/>
+        <v>244</v>
+      </c>
+      <c r="AO25" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="B26" s="2">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="2"/>
+        <v>452</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="3"/>
+        <v>582</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="4"/>
+        <v>604</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="40"/>
+        <v>658</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="6"/>
+        <v>676</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="7"/>
+        <v>684</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="8"/>
+        <v>684</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="9"/>
+        <v>720</v>
+      </c>
+      <c r="K26" s="2">
+        <f t="shared" si="10"/>
+        <v>720</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="11"/>
+        <v>742</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="12"/>
+        <v>742</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="13"/>
+        <v>742</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="14"/>
+        <v>744</v>
+      </c>
+      <c r="P26" s="2">
+        <f t="shared" si="15"/>
+        <v>870</v>
+      </c>
+      <c r="Q26" s="2">
+        <f t="shared" si="16"/>
+        <v>870</v>
+      </c>
+      <c r="R26" s="2">
+        <f t="shared" si="17"/>
+        <v>930</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="18"/>
+        <v>1002</v>
+      </c>
+      <c r="T26" s="7">
+        <f t="shared" si="19"/>
+        <v>1002</v>
+      </c>
+      <c r="V26" s="6">
+        <f t="shared" si="20"/>
+        <v>198</v>
+      </c>
+      <c r="W26" s="2">
+        <f t="shared" si="21"/>
+        <v>166</v>
+      </c>
+      <c r="X26" s="2">
+        <f t="shared" si="22"/>
+        <v>166</v>
+      </c>
+      <c r="Y26" s="2">
+        <f t="shared" si="23"/>
+        <v>188</v>
+      </c>
+      <c r="Z26" s="7">
+        <f t="shared" si="24"/>
+        <v>176</v>
+      </c>
+      <c r="AA26" s="2">
+        <f t="shared" si="41"/>
+        <v>200</v>
+      </c>
+      <c r="AB26" s="2">
+        <f t="shared" si="26"/>
+        <v>164</v>
+      </c>
+      <c r="AC26" s="2">
+        <f t="shared" si="27"/>
+        <v>164</v>
+      </c>
+      <c r="AD26" s="2">
+        <f t="shared" si="28"/>
+        <v>164</v>
+      </c>
+      <c r="AE26" s="2">
+        <f t="shared" si="29"/>
+        <v>200</v>
+      </c>
+      <c r="AF26" s="2">
+        <f t="shared" si="30"/>
+        <v>190</v>
+      </c>
+      <c r="AG26" s="2">
+        <f t="shared" si="31"/>
+        <v>194</v>
+      </c>
+      <c r="AH26" s="2">
+        <f t="shared" si="32"/>
+        <v>194</v>
+      </c>
+      <c r="AI26" s="2">
+        <f t="shared" si="33"/>
+        <v>194</v>
+      </c>
+      <c r="AJ26" s="2">
+        <f t="shared" si="34"/>
+        <v>194</v>
+      </c>
+      <c r="AK26" s="2">
+        <f t="shared" si="35"/>
+        <v>244</v>
+      </c>
+      <c r="AL26" s="2">
+        <f t="shared" si="36"/>
+        <v>244</v>
+      </c>
+      <c r="AM26" s="2">
+        <f t="shared" si="37"/>
+        <v>276</v>
+      </c>
+      <c r="AN26" s="2">
+        <f t="shared" si="38"/>
+        <v>276</v>
+      </c>
+      <c r="AO26" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <f t="shared" si="0"/>
+        <v>198</v>
+      </c>
+      <c r="B27" s="2">
+        <f t="shared" si="1"/>
+        <v>218</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="2"/>
+        <v>452</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="3"/>
+        <v>560</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="4"/>
+        <v>574</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="40"/>
+        <v>632</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="6"/>
+        <v>640</v>
+      </c>
+      <c r="H27" s="9">
+        <f>G27 + H5 * MOD(H5 + 1,2)</f>
+        <v>684</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" ref="I27:O27" si="42">H27 + I5 * MOD(I5 + 1,2)</f>
+        <v>684</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" si="42"/>
+        <v>684</v>
+      </c>
+      <c r="K27" s="9">
+        <f t="shared" si="42"/>
+        <v>684</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" si="42"/>
+        <v>738</v>
+      </c>
+      <c r="M27" s="9">
+        <f t="shared" si="42"/>
+        <v>738</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="42"/>
+        <v>738</v>
+      </c>
+      <c r="O27" s="9">
+        <f t="shared" si="42"/>
+        <v>744</v>
+      </c>
+      <c r="P27" s="2">
+        <f t="shared" si="15"/>
+        <v>820</v>
+      </c>
+      <c r="Q27" s="2">
+        <f t="shared" si="16"/>
+        <v>842</v>
+      </c>
+      <c r="R27" s="2">
+        <f t="shared" si="17"/>
+        <v>898</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="18"/>
+        <v>1002</v>
+      </c>
+      <c r="T27" s="7">
+        <f t="shared" si="19"/>
+        <v>1002</v>
+      </c>
+      <c r="V27" s="6">
+        <f t="shared" si="20"/>
+        <v>198</v>
+      </c>
+      <c r="W27" s="2">
+        <f t="shared" si="21"/>
+        <v>166</v>
+      </c>
+      <c r="X27" s="2">
+        <f t="shared" si="22"/>
+        <v>220</v>
+      </c>
+      <c r="Y27" s="2">
+        <f t="shared" si="23"/>
+        <v>188</v>
+      </c>
+      <c r="Z27" s="7">
+        <f t="shared" si="24"/>
+        <v>154</v>
+      </c>
+      <c r="AA27" s="2">
+        <f t="shared" si="41"/>
+        <v>174</v>
+      </c>
+      <c r="AB27" s="2">
+        <f t="shared" si="26"/>
+        <v>146</v>
+      </c>
+      <c r="AC27" s="9">
+        <f>AB27 + H5 * MOD(H5 + 1,2)</f>
+        <v>190</v>
+      </c>
+      <c r="AD27" s="9">
+        <f t="shared" ref="AD27:AJ27" si="43">AC27 + I5 * MOD(I5 + 1,2)</f>
+        <v>190</v>
+      </c>
+      <c r="AE27" s="9">
+        <f t="shared" si="43"/>
+        <v>190</v>
+      </c>
+      <c r="AF27" s="9">
+        <f t="shared" si="43"/>
+        <v>190</v>
+      </c>
+      <c r="AG27" s="9">
+        <f t="shared" si="43"/>
+        <v>244</v>
+      </c>
+      <c r="AH27" s="9">
+        <f t="shared" si="43"/>
+        <v>244</v>
+      </c>
+      <c r="AI27" s="9">
+        <f t="shared" si="43"/>
+        <v>244</v>
+      </c>
+      <c r="AJ27" s="9">
+        <f t="shared" si="43"/>
+        <v>250</v>
+      </c>
+      <c r="AK27" s="2">
+        <f t="shared" si="35"/>
+        <v>304</v>
+      </c>
+      <c r="AL27" s="2">
+        <f t="shared" si="36"/>
+        <v>310</v>
+      </c>
+      <c r="AM27" s="2">
+        <f t="shared" si="37"/>
+        <v>300</v>
+      </c>
+      <c r="AN27" s="2">
+        <f t="shared" si="38"/>
+        <v>320</v>
+      </c>
+      <c r="AO27" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="B28" s="2">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="2"/>
+        <v>394</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="3"/>
+        <v>534</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="4"/>
+        <v>574</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="40"/>
+        <v>598</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="6"/>
+        <v>634</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="7"/>
+        <v>690</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="8"/>
+        <v>756</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="K28" s="2">
+        <f t="shared" si="10"/>
+        <v>830</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" si="11"/>
+        <v>852</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="12"/>
+        <v>852</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="13"/>
+        <v>852</v>
+      </c>
+      <c r="O28" s="7">
+        <f t="shared" si="14"/>
+        <v>896</v>
+      </c>
+      <c r="P28" s="2">
+        <f t="shared" ref="P28:P36" si="44">P29 + P6 * MOD(P6 + 1,2)</f>
+        <v>766</v>
+      </c>
+      <c r="Q28" s="2">
+        <f t="shared" si="16"/>
+        <v>768</v>
+      </c>
+      <c r="R28" s="2">
+        <f t="shared" si="17"/>
+        <v>898</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="18"/>
+        <v>982</v>
+      </c>
+      <c r="T28" s="7">
+        <f t="shared" si="19"/>
+        <v>982</v>
+      </c>
+      <c r="V28" s="6">
+        <f t="shared" si="20"/>
+        <v>178</v>
+      </c>
+      <c r="W28" s="2">
+        <f t="shared" si="21"/>
+        <v>154</v>
+      </c>
+      <c r="X28" s="2">
+        <f t="shared" si="22"/>
+        <v>162</v>
+      </c>
+      <c r="Y28" s="2">
+        <f t="shared" si="23"/>
+        <v>162</v>
+      </c>
+      <c r="Z28" s="7">
+        <f t="shared" si="24"/>
+        <v>154</v>
+      </c>
+      <c r="AA28" s="2">
+        <f t="shared" si="41"/>
+        <v>140</v>
+      </c>
+      <c r="AB28" s="2">
+        <f t="shared" si="26"/>
+        <v>140</v>
+      </c>
+      <c r="AC28" s="2">
+        <f t="shared" si="27"/>
+        <v>166</v>
+      </c>
+      <c r="AD28" s="2">
+        <f t="shared" si="28"/>
+        <v>186</v>
+      </c>
+      <c r="AE28" s="2">
+        <f t="shared" si="29"/>
+        <v>186</v>
+      </c>
+      <c r="AF28" s="2">
+        <f t="shared" si="30"/>
+        <v>184</v>
+      </c>
+      <c r="AG28" s="2">
+        <f t="shared" si="31"/>
+        <v>158</v>
+      </c>
+      <c r="AH28" s="2">
+        <f t="shared" si="32"/>
+        <v>144</v>
+      </c>
+      <c r="AI28" s="2">
+        <f t="shared" si="33"/>
+        <v>144</v>
+      </c>
+      <c r="AJ28" s="7">
+        <f t="shared" si="34"/>
+        <v>144</v>
+      </c>
+      <c r="AK28" s="2">
+        <f t="shared" ref="AK28:AK36" si="45">AK29 + P6 * MOD(P6 + 1,2)</f>
+        <v>396</v>
+      </c>
+      <c r="AL28" s="2">
+        <f t="shared" si="36"/>
+        <v>288</v>
+      </c>
+      <c r="AM28" s="2">
+        <f t="shared" si="37"/>
+        <v>300</v>
+      </c>
+      <c r="AN28" s="2">
+        <f t="shared" si="38"/>
+        <v>304</v>
+      </c>
+      <c r="AO28" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="B29" s="2">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="2"/>
+        <v>340</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="3"/>
+        <v>534</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="4"/>
+        <v>534</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="40"/>
+        <v>598</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="6"/>
+        <v>634</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="7"/>
+        <v>664</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="8"/>
+        <v>714</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" si="10"/>
+        <v>830</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="11"/>
+        <v>838</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="12"/>
+        <v>838</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="13"/>
+        <v>842</v>
+      </c>
+      <c r="O29" s="7">
+        <f t="shared" si="14"/>
+        <v>896</v>
+      </c>
+      <c r="P29" s="2">
+        <f t="shared" si="44"/>
+        <v>732</v>
+      </c>
+      <c r="Q29" s="2">
+        <f t="shared" si="16"/>
+        <v>756</v>
+      </c>
+      <c r="R29" s="2">
+        <f t="shared" si="17"/>
+        <v>884</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="18"/>
+        <v>978</v>
+      </c>
+      <c r="T29" s="7">
+        <f t="shared" si="19"/>
+        <v>978</v>
+      </c>
+      <c r="V29" s="6">
+        <f t="shared" si="20"/>
+        <v>178</v>
+      </c>
+      <c r="W29" s="2">
+        <f t="shared" si="21"/>
+        <v>154</v>
+      </c>
+      <c r="X29" s="2">
+        <f t="shared" si="22"/>
+        <v>108</v>
+      </c>
+      <c r="Y29" s="2">
+        <f t="shared" si="23"/>
+        <v>166</v>
+      </c>
+      <c r="Z29" s="7">
+        <f t="shared" si="24"/>
+        <v>114</v>
+      </c>
+      <c r="AA29" s="2">
+        <f t="shared" si="41"/>
+        <v>140</v>
+      </c>
+      <c r="AB29" s="2">
+        <f t="shared" si="26"/>
+        <v>144</v>
+      </c>
+      <c r="AC29" s="2">
+        <f t="shared" si="27"/>
+        <v>144</v>
+      </c>
+      <c r="AD29" s="2">
+        <f t="shared" si="28"/>
+        <v>144</v>
+      </c>
+      <c r="AE29" s="2">
+        <f t="shared" si="29"/>
+        <v>198</v>
+      </c>
+      <c r="AF29" s="2">
+        <f t="shared" si="30"/>
+        <v>184</v>
+      </c>
+      <c r="AG29" s="2">
+        <f t="shared" si="31"/>
+        <v>144</v>
+      </c>
+      <c r="AH29" s="2">
+        <f t="shared" si="32"/>
+        <v>144</v>
+      </c>
+      <c r="AI29" s="2">
+        <f t="shared" si="33"/>
+        <v>144</v>
+      </c>
+      <c r="AJ29" s="7">
+        <f t="shared" si="34"/>
+        <v>198</v>
+      </c>
+      <c r="AK29" s="2">
+        <f t="shared" si="45"/>
+        <v>362</v>
+      </c>
+      <c r="AL29" s="2">
+        <f t="shared" si="36"/>
+        <v>286</v>
+      </c>
+      <c r="AM29" s="2">
+        <f t="shared" si="37"/>
+        <v>286</v>
+      </c>
+      <c r="AN29" s="2">
+        <f t="shared" si="38"/>
+        <v>332</v>
+      </c>
+      <c r="AO29" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="B30" s="2">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="2"/>
+        <v>340</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="3"/>
+        <v>476</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="4"/>
+        <v>476</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="40"/>
+        <v>592</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="6"/>
+        <v>630</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="7"/>
+        <v>664</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="8"/>
+        <v>714</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="9"/>
+        <v>746</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="10"/>
+        <v>746</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="11"/>
+        <v>746</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="12"/>
+        <v>810</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="13"/>
+        <v>842</v>
+      </c>
+      <c r="O30" s="7">
+        <f t="shared" si="14"/>
+        <v>842</v>
+      </c>
+      <c r="P30" s="2">
+        <f t="shared" si="44"/>
+        <v>732</v>
+      </c>
+      <c r="Q30" s="2">
+        <f t="shared" si="16"/>
+        <v>756</v>
+      </c>
+      <c r="R30" s="2">
+        <f t="shared" si="17"/>
+        <v>884</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="18"/>
+        <v>932</v>
+      </c>
+      <c r="T30" s="7">
+        <f t="shared" si="19"/>
+        <v>932</v>
+      </c>
+      <c r="V30" s="6">
+        <f t="shared" si="20"/>
+        <v>156</v>
+      </c>
+      <c r="W30" s="2">
+        <f t="shared" si="21"/>
+        <v>154</v>
+      </c>
+      <c r="X30" s="2">
+        <f t="shared" si="22"/>
+        <v>108</v>
+      </c>
+      <c r="Y30" s="2">
+        <f t="shared" si="23"/>
+        <v>158</v>
+      </c>
+      <c r="Z30" s="7">
+        <f t="shared" si="24"/>
+        <v>114</v>
+      </c>
+      <c r="AA30" s="2">
+        <f t="shared" si="41"/>
+        <v>134</v>
+      </c>
+      <c r="AB30" s="2">
+        <f t="shared" si="26"/>
+        <v>152</v>
+      </c>
+      <c r="AC30" s="2">
+        <f t="shared" si="27"/>
+        <v>150</v>
+      </c>
+      <c r="AD30" s="2">
+        <f t="shared" si="28"/>
+        <v>186</v>
+      </c>
+      <c r="AE30" s="2">
+        <f t="shared" si="29"/>
+        <v>206</v>
+      </c>
+      <c r="AF30" s="2">
+        <f t="shared" si="30"/>
+        <v>154</v>
+      </c>
+      <c r="AG30" s="2">
+        <f t="shared" si="31"/>
+        <v>136</v>
+      </c>
+      <c r="AH30" s="2">
+        <f t="shared" si="32"/>
+        <v>186</v>
+      </c>
+      <c r="AI30" s="2">
+        <f t="shared" si="33"/>
+        <v>196</v>
+      </c>
+      <c r="AJ30" s="7">
+        <f t="shared" si="34"/>
+        <v>164</v>
+      </c>
+      <c r="AK30" s="2">
+        <f t="shared" si="45"/>
+        <v>362</v>
+      </c>
+      <c r="AL30" s="2">
+        <f t="shared" si="36"/>
+        <v>286</v>
+      </c>
+      <c r="AM30" s="2">
+        <f t="shared" si="37"/>
+        <v>342</v>
+      </c>
+      <c r="AN30" s="2">
+        <f t="shared" si="38"/>
+        <v>304</v>
+      </c>
+      <c r="AO30" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="B31" s="2">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="3"/>
+        <v>422</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="4"/>
+        <v>470</v>
+      </c>
+      <c r="F31" s="2">
+        <f>F32 + F9 * MOD(F9 + 1,2)</f>
+        <v>592</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="6"/>
+        <v>612</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="7"/>
+        <v>650</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="8"/>
+        <v>654</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="9"/>
+        <v>696</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="10"/>
+        <v>714</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="11"/>
+        <v>714</v>
+      </c>
+      <c r="M31" s="2">
+        <f t="shared" si="12"/>
+        <v>760</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="13"/>
+        <v>784</v>
+      </c>
+      <c r="O31" s="7">
+        <f t="shared" si="14"/>
+        <v>810</v>
+      </c>
+      <c r="P31" s="2">
+        <f t="shared" si="44"/>
+        <v>732</v>
+      </c>
+      <c r="Q31" s="2">
+        <f t="shared" si="16"/>
+        <v>756</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" si="17"/>
+        <v>828</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="18"/>
+        <v>864</v>
+      </c>
+      <c r="T31" s="7">
+        <f t="shared" si="19"/>
+        <v>864</v>
+      </c>
+      <c r="V31" s="6">
+        <f t="shared" si="20"/>
+        <v>156</v>
+      </c>
+      <c r="W31" s="2">
+        <f t="shared" si="21"/>
+        <v>154</v>
+      </c>
+      <c r="X31" s="2">
+        <f t="shared" si="22"/>
+        <v>104</v>
+      </c>
+      <c r="Y31" s="2">
+        <f t="shared" si="23"/>
+        <v>104</v>
+      </c>
+      <c r="Z31" s="7">
+        <f t="shared" si="24"/>
+        <v>114</v>
+      </c>
+      <c r="AA31" s="2">
+        <f>AA32 + F9 * MOD(F9 + 1,2)</f>
+        <v>134</v>
+      </c>
+      <c r="AB31" s="2">
+        <f t="shared" si="26"/>
+        <v>136</v>
+      </c>
+      <c r="AC31" s="2">
+        <f t="shared" si="27"/>
+        <v>136</v>
+      </c>
+      <c r="AD31" s="2">
+        <f t="shared" si="28"/>
+        <v>136</v>
+      </c>
+      <c r="AE31" s="2">
+        <f t="shared" si="29"/>
+        <v>174</v>
+      </c>
+      <c r="AF31" s="2">
+        <f t="shared" si="30"/>
+        <v>154</v>
+      </c>
+      <c r="AG31" s="2">
+        <f t="shared" si="31"/>
+        <v>136</v>
+      </c>
+      <c r="AH31" s="2">
+        <f t="shared" si="32"/>
+        <v>164</v>
+      </c>
+      <c r="AI31" s="2">
+        <f t="shared" si="33"/>
+        <v>164</v>
+      </c>
+      <c r="AJ31" s="7">
+        <f t="shared" si="34"/>
+        <v>164</v>
+      </c>
+      <c r="AK31" s="2">
+        <f t="shared" si="45"/>
+        <v>362</v>
+      </c>
+      <c r="AL31" s="2">
+        <f t="shared" si="36"/>
+        <v>286</v>
+      </c>
+      <c r="AM31" s="2">
+        <f t="shared" si="37"/>
+        <v>292</v>
+      </c>
+      <c r="AN31" s="2">
+        <f t="shared" si="38"/>
+        <v>256</v>
+      </c>
+      <c r="AO31" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="B32" s="2">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="3"/>
+        <v>422</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="4"/>
+        <v>460</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="5"/>
+        <v>592</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="6"/>
+        <v>610</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="7"/>
+        <v>650</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="8"/>
+        <v>654</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="9"/>
+        <v>658</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="10"/>
+        <v>658</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="11"/>
+        <v>694</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="12"/>
+        <v>732</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="13"/>
+        <v>784</v>
+      </c>
+      <c r="O32" s="7">
+        <f t="shared" si="14"/>
+        <v>810</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" si="44"/>
+        <v>690</v>
+      </c>
+      <c r="Q32" s="2">
+        <f t="shared" si="16"/>
+        <v>756</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="17"/>
+        <v>772</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="18"/>
+        <v>772</v>
+      </c>
+      <c r="T32" s="7">
+        <f t="shared" si="19"/>
+        <v>780</v>
+      </c>
+      <c r="V32" s="6">
+        <f t="shared" si="20"/>
+        <v>156</v>
+      </c>
+      <c r="W32" s="2">
+        <f t="shared" si="21"/>
+        <v>154</v>
+      </c>
+      <c r="X32" s="2">
+        <f t="shared" si="22"/>
+        <v>104</v>
+      </c>
+      <c r="Y32" s="2">
+        <f t="shared" si="23"/>
+        <v>110</v>
+      </c>
+      <c r="Z32" s="2">
+        <f t="shared" si="24"/>
+        <v>112</v>
+      </c>
+      <c r="AA32" s="2">
+        <f t="shared" si="25"/>
+        <v>134</v>
+      </c>
+      <c r="AB32" s="2">
+        <f t="shared" si="26"/>
+        <v>134</v>
+      </c>
+      <c r="AC32" s="2">
+        <f t="shared" si="27"/>
+        <v>174</v>
+      </c>
+      <c r="AD32" s="2">
+        <f t="shared" si="28"/>
+        <v>160</v>
+      </c>
+      <c r="AE32" s="2">
+        <f t="shared" si="29"/>
+        <v>136</v>
+      </c>
+      <c r="AF32" s="2">
+        <f t="shared" si="30"/>
+        <v>136</v>
+      </c>
+      <c r="AG32" s="2">
+        <f t="shared" si="31"/>
+        <v>136</v>
+      </c>
+      <c r="AH32" s="2">
+        <f t="shared" si="32"/>
+        <v>152</v>
+      </c>
+      <c r="AI32" s="2">
+        <f t="shared" si="33"/>
+        <v>164</v>
+      </c>
+      <c r="AJ32" s="7">
+        <f t="shared" si="34"/>
+        <v>190</v>
+      </c>
+      <c r="AK32" s="2">
+        <f t="shared" si="45"/>
+        <v>320</v>
+      </c>
+      <c r="AL32" s="2">
+        <f t="shared" si="36"/>
+        <v>286</v>
+      </c>
+      <c r="AM32" s="2">
+        <f t="shared" si="37"/>
+        <v>236</v>
+      </c>
+      <c r="AN32" s="2">
+        <f t="shared" si="38"/>
+        <v>220</v>
+      </c>
+      <c r="AO32" s="7">
+        <f t="shared" si="39"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="B33" s="2">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="3"/>
+        <v>416</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="4"/>
+        <v>458</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="5"/>
+        <v>570</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="6"/>
+        <v>610</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="7"/>
+        <v>610</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="8"/>
+        <v>610</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="9"/>
+        <v>610</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="10"/>
+        <v>648</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="11"/>
+        <v>694</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" si="12"/>
+        <v>716</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="13"/>
+        <v>772</v>
+      </c>
+      <c r="O33" s="7">
+        <f t="shared" si="14"/>
+        <v>772</v>
+      </c>
+      <c r="P33" s="2">
+        <f t="shared" si="44"/>
+        <v>690</v>
+      </c>
+      <c r="Q33" s="2">
+        <f t="shared" si="16"/>
+        <v>706</v>
+      </c>
+      <c r="R33" s="2">
+        <f t="shared" si="17"/>
+        <v>706</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="18"/>
+        <v>708</v>
+      </c>
+      <c r="T33" s="7">
+        <f t="shared" si="19"/>
+        <v>714</v>
+      </c>
+      <c r="V33" s="6">
+        <f t="shared" si="20"/>
+        <v>156</v>
+      </c>
+      <c r="W33" s="2">
+        <f t="shared" si="21"/>
+        <v>104</v>
+      </c>
+      <c r="X33" s="2">
+        <f t="shared" si="22"/>
+        <v>104</v>
+      </c>
+      <c r="Y33" s="2">
+        <f t="shared" si="23"/>
+        <v>104</v>
+      </c>
+      <c r="Z33" s="2">
+        <f t="shared" si="24"/>
+        <v>120</v>
+      </c>
+      <c r="AA33" s="2">
+        <f t="shared" si="25"/>
+        <v>176</v>
+      </c>
+      <c r="AB33" s="2">
+        <f t="shared" si="26"/>
+        <v>210</v>
+      </c>
+      <c r="AC33" s="2">
+        <f t="shared" si="27"/>
+        <v>166</v>
+      </c>
+      <c r="AD33" s="2">
+        <f t="shared" si="28"/>
+        <v>156</v>
+      </c>
+      <c r="AE33" s="2">
+        <f t="shared" si="29"/>
+        <v>132</v>
+      </c>
+      <c r="AF33" s="2">
+        <f t="shared" si="30"/>
+        <v>154</v>
+      </c>
+      <c r="AG33" s="2">
+        <f t="shared" si="31"/>
+        <v>178</v>
+      </c>
+      <c r="AH33" s="2">
+        <f t="shared" si="32"/>
+        <v>166</v>
+      </c>
+      <c r="AI33" s="2">
+        <f t="shared" si="33"/>
+        <v>200</v>
+      </c>
+      <c r="AJ33" s="7">
+        <f t="shared" si="34"/>
+        <v>180</v>
+      </c>
+      <c r="AK33" s="2">
+        <f t="shared" si="45"/>
+        <v>320</v>
+      </c>
+      <c r="AL33" s="2">
+        <f t="shared" si="36"/>
+        <v>236</v>
+      </c>
+      <c r="AM33" s="2">
+        <f t="shared" si="37"/>
+        <v>220</v>
+      </c>
+      <c r="AN33" s="2">
+        <f t="shared" si="38"/>
+        <v>220</v>
+      </c>
+      <c r="AO33" s="7">
+        <f t="shared" si="39"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="B34" s="2">
+        <f t="shared" si="1"/>
+        <v>156</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="3"/>
+        <v>416</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="4"/>
+        <v>442</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="5"/>
+        <v>514</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="6"/>
+        <v>556</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="7"/>
+        <v>574</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="8"/>
+        <v>574</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="9"/>
+        <v>574</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="10"/>
+        <v>626</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="11"/>
+        <v>626</v>
+      </c>
+      <c r="M34" s="2">
+        <f t="shared" si="12"/>
+        <v>638</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="13"/>
+        <v>638</v>
+      </c>
+      <c r="O34" s="7">
+        <f t="shared" si="14"/>
+        <v>674</v>
+      </c>
+      <c r="P34" s="2">
+        <f t="shared" si="44"/>
+        <v>684</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" si="16"/>
+        <v>684</v>
+      </c>
+      <c r="R34" s="2">
+        <f t="shared" si="17"/>
+        <v>684</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="18"/>
+        <v>708</v>
+      </c>
+      <c r="T34" s="7">
+        <f t="shared" si="19"/>
+        <v>714</v>
+      </c>
+      <c r="V34" s="6">
+        <f t="shared" si="20"/>
+        <v>156</v>
+      </c>
+      <c r="W34" s="2">
+        <f t="shared" si="21"/>
+        <v>104</v>
+      </c>
+      <c r="X34" s="2">
+        <f t="shared" si="22"/>
+        <v>104</v>
+      </c>
+      <c r="Y34" s="2">
+        <f t="shared" si="23"/>
+        <v>154</v>
+      </c>
+      <c r="Z34" s="2">
+        <f t="shared" si="24"/>
+        <v>154</v>
+      </c>
+      <c r="AA34" s="2">
+        <f t="shared" si="25"/>
+        <v>200</v>
+      </c>
+      <c r="AB34" s="2">
+        <f t="shared" si="26"/>
+        <v>170</v>
+      </c>
+      <c r="AC34" s="2">
+        <f t="shared" si="27"/>
+        <v>166</v>
+      </c>
+      <c r="AD34" s="2">
+        <f t="shared" si="28"/>
+        <v>156</v>
+      </c>
+      <c r="AE34" s="2">
+        <f t="shared" si="29"/>
+        <v>132</v>
+      </c>
+      <c r="AF34" s="2">
+        <f t="shared" si="30"/>
+        <v>184</v>
+      </c>
+      <c r="AG34" s="2">
+        <f t="shared" si="31"/>
+        <v>132</v>
+      </c>
+      <c r="AH34" s="2">
+        <f t="shared" si="32"/>
+        <v>144</v>
+      </c>
+      <c r="AI34" s="2">
+        <f t="shared" si="33"/>
+        <v>144</v>
+      </c>
+      <c r="AJ34" s="7">
+        <f t="shared" si="34"/>
+        <v>180</v>
+      </c>
+      <c r="AK34" s="2">
+        <f t="shared" si="45"/>
+        <v>314</v>
+      </c>
+      <c r="AL34" s="2">
+        <f t="shared" si="36"/>
+        <v>220</v>
+      </c>
+      <c r="AM34" s="2">
+        <f t="shared" si="37"/>
+        <v>220</v>
+      </c>
+      <c r="AN34" s="2">
+        <f t="shared" si="38"/>
+        <v>220</v>
+      </c>
+      <c r="AO34" s="7">
+        <f t="shared" si="39"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+      <c r="B35" s="2">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="3"/>
+        <v>366</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="4"/>
+        <v>442</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="5"/>
+        <v>458</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="6"/>
+        <v>458</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="7"/>
+        <v>534</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="8"/>
+        <v>558</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="9"/>
+        <v>558</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="10"/>
+        <v>558</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="11"/>
+        <v>558</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" si="12"/>
+        <v>586</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="13"/>
+        <v>586</v>
+      </c>
+      <c r="O35" s="7">
+        <f t="shared" si="14"/>
+        <v>594</v>
+      </c>
+      <c r="P35" s="2">
+        <f t="shared" si="44"/>
+        <v>642</v>
+      </c>
+      <c r="Q35" s="2">
+        <f t="shared" si="16"/>
+        <v>642</v>
+      </c>
+      <c r="R35" s="2">
+        <f t="shared" si="17"/>
+        <v>672</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="18"/>
+        <v>708</v>
+      </c>
+      <c r="T35" s="7">
+        <f t="shared" si="19"/>
+        <v>708</v>
+      </c>
+      <c r="V35" s="6">
+        <f t="shared" si="20"/>
+        <v>154</v>
+      </c>
+      <c r="W35" s="2">
+        <f t="shared" si="21"/>
+        <v>104</v>
+      </c>
+      <c r="X35" s="2">
+        <f t="shared" si="22"/>
+        <v>104</v>
+      </c>
+      <c r="Y35" s="2">
+        <f t="shared" si="23"/>
+        <v>126</v>
+      </c>
+      <c r="Z35" s="2">
+        <f t="shared" si="24"/>
+        <v>168</v>
+      </c>
+      <c r="AA35" s="2">
+        <f t="shared" si="25"/>
+        <v>144</v>
+      </c>
+      <c r="AB35" s="2">
+        <f t="shared" si="26"/>
+        <v>128</v>
+      </c>
+      <c r="AC35" s="2">
+        <f t="shared" si="27"/>
+        <v>148</v>
+      </c>
+      <c r="AD35" s="2">
+        <f t="shared" si="28"/>
+        <v>156</v>
+      </c>
+      <c r="AE35" s="2">
+        <f t="shared" si="29"/>
+        <v>132</v>
+      </c>
+      <c r="AF35" s="2">
+        <f t="shared" si="30"/>
+        <v>132</v>
+      </c>
+      <c r="AG35" s="2">
+        <f t="shared" si="31"/>
+        <v>132</v>
+      </c>
+      <c r="AH35" s="2">
+        <f t="shared" si="32"/>
+        <v>160</v>
+      </c>
+      <c r="AI35" s="2">
+        <f t="shared" si="33"/>
+        <v>160</v>
+      </c>
+      <c r="AJ35" s="7">
+        <f t="shared" si="34"/>
+        <v>168</v>
+      </c>
+      <c r="AK35" s="2">
+        <f t="shared" si="45"/>
+        <v>272</v>
+      </c>
+      <c r="AL35" s="2">
+        <f t="shared" si="36"/>
+        <v>220</v>
+      </c>
+      <c r="AM35" s="2">
+        <f t="shared" si="37"/>
+        <v>250</v>
+      </c>
+      <c r="AN35" s="2">
+        <f t="shared" si="38"/>
+        <v>266</v>
+      </c>
+      <c r="AO35" s="7">
+        <f t="shared" si="39"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="B36" s="2">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="3"/>
+        <v>344</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="5"/>
+        <v>406</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="6"/>
+        <v>448</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="7"/>
+        <v>514</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="8"/>
+        <v>514</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="9"/>
+        <v>514</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="10"/>
+        <v>514</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="11"/>
+        <v>514</v>
+      </c>
+      <c r="M36" s="2">
+        <f t="shared" si="12"/>
+        <v>514</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="13"/>
+        <v>578</v>
+      </c>
+      <c r="O36" s="7">
+        <f t="shared" si="14"/>
+        <v>578</v>
+      </c>
+      <c r="P36" s="2">
+        <f t="shared" si="44"/>
+        <v>642</v>
+      </c>
+      <c r="Q36" s="2">
+        <f t="shared" si="16"/>
+        <v>642</v>
+      </c>
+      <c r="R36" s="2">
+        <f t="shared" si="17"/>
+        <v>642</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="18"/>
+        <v>658</v>
+      </c>
+      <c r="T36" s="7">
+        <f t="shared" si="19"/>
+        <v>680</v>
+      </c>
+      <c r="V36" s="6">
+        <f t="shared" si="20"/>
+        <v>112</v>
+      </c>
+      <c r="W36" s="2">
+        <f t="shared" si="21"/>
+        <v>104</v>
+      </c>
+      <c r="X36" s="2">
+        <f t="shared" si="22"/>
+        <v>154</v>
+      </c>
+      <c r="Y36" s="2">
+        <f t="shared" si="23"/>
+        <v>154</v>
+      </c>
+      <c r="Z36" s="2">
+        <f t="shared" si="24"/>
+        <v>154</v>
+      </c>
+      <c r="AA36" s="2">
+        <f t="shared" si="25"/>
+        <v>128</v>
+      </c>
+      <c r="AB36" s="2">
+        <f t="shared" si="26"/>
+        <v>128</v>
+      </c>
+      <c r="AC36" s="2">
+        <f t="shared" si="27"/>
+        <v>180</v>
+      </c>
+      <c r="AD36" s="2">
+        <f t="shared" si="28"/>
+        <v>132</v>
+      </c>
+      <c r="AE36" s="2">
+        <f t="shared" si="29"/>
+        <v>132</v>
+      </c>
+      <c r="AF36" s="2">
+        <f t="shared" si="30"/>
+        <v>132</v>
+      </c>
+      <c r="AG36" s="2">
+        <f t="shared" si="31"/>
+        <v>132</v>
+      </c>
+      <c r="AH36" s="2">
+        <f t="shared" si="32"/>
+        <v>132</v>
+      </c>
+      <c r="AI36" s="2">
+        <f t="shared" si="33"/>
+        <v>174</v>
+      </c>
+      <c r="AJ36" s="7">
+        <f t="shared" si="34"/>
+        <v>170</v>
+      </c>
+      <c r="AK36" s="2">
+        <f t="shared" si="45"/>
+        <v>272</v>
+      </c>
+      <c r="AL36" s="2">
+        <f t="shared" si="36"/>
+        <v>220</v>
+      </c>
+      <c r="AM36" s="2">
+        <f t="shared" si="37"/>
+        <v>220</v>
+      </c>
+      <c r="AN36" s="2">
+        <f t="shared" si="38"/>
+        <v>230</v>
+      </c>
+      <c r="AO36" s="7">
+        <f t="shared" si="39"/>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="B37" s="2">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="2"/>
+        <v>286</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="3"/>
+        <v>344</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="5"/>
+        <v>400</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="6"/>
+        <v>448</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="7"/>
+        <v>462</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="8"/>
+        <v>462</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="9"/>
+        <v>502</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="10"/>
+        <v>502</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="11"/>
+        <v>504</v>
+      </c>
+      <c r="M37" s="2">
+        <f t="shared" si="12"/>
+        <v>504</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="13"/>
+        <v>536</v>
+      </c>
+      <c r="O37" s="7">
+        <f t="shared" si="14"/>
+        <v>536</v>
+      </c>
+      <c r="P37" s="2">
+        <f>P38 + P15 * MOD(P15 + 1,2)</f>
+        <v>590</v>
+      </c>
+      <c r="Q37" s="2">
+        <f t="shared" si="16"/>
+        <v>590</v>
+      </c>
+      <c r="R37" s="2">
+        <f t="shared" si="17"/>
+        <v>634</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="18"/>
+        <v>648</v>
+      </c>
+      <c r="T37" s="7">
+        <f t="shared" si="19"/>
+        <v>652</v>
+      </c>
+      <c r="V37" s="6">
+        <f t="shared" si="20"/>
+        <v>112</v>
+      </c>
+      <c r="W37" s="2">
+        <f t="shared" si="21"/>
+        <v>104</v>
+      </c>
+      <c r="X37" s="2">
+        <f t="shared" si="22"/>
+        <v>158</v>
+      </c>
+      <c r="Y37" s="2">
+        <f t="shared" si="23"/>
+        <v>174</v>
+      </c>
+      <c r="Z37" s="2">
+        <f t="shared" si="24"/>
+        <v>172</v>
+      </c>
+      <c r="AA37" s="2">
+        <f t="shared" si="25"/>
+        <v>122</v>
+      </c>
+      <c r="AB37" s="2">
+        <f t="shared" si="26"/>
+        <v>166</v>
+      </c>
+      <c r="AC37" s="2">
+        <f t="shared" si="27"/>
+        <v>132</v>
+      </c>
+      <c r="AD37" s="2">
+        <f t="shared" si="28"/>
+        <v>132</v>
+      </c>
+      <c r="AE37" s="2">
+        <f t="shared" si="29"/>
+        <v>172</v>
+      </c>
+      <c r="AF37" s="2">
+        <f t="shared" si="30"/>
+        <v>172</v>
+      </c>
+      <c r="AG37" s="2">
+        <f t="shared" si="31"/>
+        <v>174</v>
+      </c>
+      <c r="AH37" s="2">
+        <f t="shared" si="32"/>
+        <v>170</v>
+      </c>
+      <c r="AI37" s="2">
+        <f t="shared" si="33"/>
+        <v>202</v>
+      </c>
+      <c r="AJ37" s="7">
+        <f t="shared" si="34"/>
+        <v>170</v>
+      </c>
+      <c r="AK37" s="2">
+        <f>AK38 + P15 * MOD(P15 + 1,2)</f>
+        <v>220</v>
+      </c>
+      <c r="AL37" s="2">
+        <f t="shared" si="36"/>
+        <v>220</v>
+      </c>
+      <c r="AM37" s="2">
+        <f t="shared" si="37"/>
+        <v>264</v>
+      </c>
+      <c r="AN37" s="2">
+        <f t="shared" si="38"/>
+        <v>264</v>
+      </c>
+      <c r="AO37" s="7">
+        <f t="shared" si="39"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="B38" s="2">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="2"/>
+        <v>232</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="3"/>
+        <v>232</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="4"/>
+        <v>234</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="5"/>
+        <v>254</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="6"/>
+        <v>276</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="7"/>
+        <v>326</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="8"/>
+        <v>378</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="9"/>
+        <v>378</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="10"/>
+        <v>394</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="11"/>
+        <v>402</v>
+      </c>
+      <c r="M38" s="2">
+        <f t="shared" si="12"/>
+        <v>418</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="13"/>
+        <v>486</v>
+      </c>
+      <c r="O38" s="2">
+        <f t="shared" si="14"/>
+        <v>486</v>
+      </c>
+      <c r="P38" s="2">
+        <f t="shared" si="15"/>
+        <v>590</v>
+      </c>
+      <c r="Q38" s="2">
+        <f t="shared" si="16"/>
+        <v>590</v>
+      </c>
+      <c r="R38" s="2">
+        <f t="shared" si="17"/>
+        <v>590</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="18"/>
+        <v>648</v>
+      </c>
+      <c r="T38" s="7">
+        <f t="shared" si="19"/>
+        <v>652</v>
+      </c>
+      <c r="V38" s="6">
+        <f t="shared" si="20"/>
+        <v>112</v>
+      </c>
+      <c r="W38" s="2">
+        <f t="shared" si="21"/>
+        <v>80</v>
+      </c>
+      <c r="X38" s="2">
+        <f t="shared" si="22"/>
+        <v>138</v>
+      </c>
+      <c r="Y38" s="2">
+        <f t="shared" si="23"/>
+        <v>116</v>
+      </c>
+      <c r="Z38" s="2">
+        <f t="shared" si="24"/>
+        <v>116</v>
+      </c>
+      <c r="AA38" s="2">
+        <f t="shared" si="25"/>
+        <v>122</v>
+      </c>
+      <c r="AB38" s="2">
+        <f t="shared" si="26"/>
+        <v>118</v>
+      </c>
+      <c r="AC38" s="2">
+        <f t="shared" si="27"/>
+        <v>118</v>
+      </c>
+      <c r="AD38" s="2">
+        <f t="shared" si="28"/>
+        <v>170</v>
+      </c>
+      <c r="AE38" s="2">
+        <f t="shared" si="29"/>
+        <v>170</v>
+      </c>
+      <c r="AF38" s="2">
+        <f t="shared" si="30"/>
+        <v>186</v>
+      </c>
+      <c r="AG38" s="2">
+        <f t="shared" si="31"/>
+        <v>178</v>
+      </c>
+      <c r="AH38" s="2">
+        <f t="shared" si="32"/>
+        <v>170</v>
+      </c>
+      <c r="AI38" s="2">
+        <f t="shared" si="33"/>
+        <v>186</v>
+      </c>
+      <c r="AJ38" s="2">
+        <f t="shared" si="34"/>
+        <v>170</v>
+      </c>
+      <c r="AK38" s="2">
+        <f t="shared" si="35"/>
+        <v>220</v>
+      </c>
+      <c r="AL38" s="2">
+        <f t="shared" si="36"/>
+        <v>220</v>
+      </c>
+      <c r="AM38" s="2">
+        <f t="shared" si="37"/>
+        <v>220</v>
+      </c>
+      <c r="AN38" s="2">
+        <f t="shared" si="38"/>
+        <v>272</v>
+      </c>
+      <c r="AO38" s="7">
+        <f t="shared" si="39"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B39" s="2">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="C39" s="2">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="3"/>
+        <v>214</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="4"/>
+        <v>234</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="5"/>
+        <v>234</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="6"/>
+        <v>264</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="7"/>
+        <v>326</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="8"/>
+        <v>326</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="9"/>
+        <v>372</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="10"/>
+        <v>372</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="11"/>
+        <v>380</v>
+      </c>
+      <c r="M39" s="2">
+        <f t="shared" si="12"/>
+        <v>418</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="13"/>
+        <v>470</v>
+      </c>
+      <c r="O39" s="2">
+        <f t="shared" si="14"/>
+        <v>470</v>
+      </c>
+      <c r="P39" s="2">
+        <f t="shared" si="15"/>
+        <v>540</v>
+      </c>
+      <c r="Q39" s="2">
+        <f t="shared" si="16"/>
+        <v>540</v>
+      </c>
+      <c r="R39" s="2">
+        <f t="shared" si="17"/>
+        <v>576</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="18"/>
+        <v>576</v>
+      </c>
+      <c r="T39" s="7">
+        <f t="shared" si="19"/>
+        <v>614</v>
+      </c>
+      <c r="V39" s="6">
+        <f t="shared" si="20"/>
+        <v>72</v>
+      </c>
+      <c r="W39" s="2">
+        <f t="shared" si="21"/>
+        <v>80</v>
+      </c>
+      <c r="X39" s="2">
+        <f t="shared" si="22"/>
+        <v>110</v>
+      </c>
+      <c r="Y39" s="2">
+        <f t="shared" si="23"/>
+        <v>116</v>
+      </c>
+      <c r="Z39" s="2">
+        <f t="shared" si="24"/>
+        <v>122</v>
+      </c>
+      <c r="AA39" s="2">
+        <f t="shared" si="25"/>
+        <v>102</v>
+      </c>
+      <c r="AB39" s="2">
+        <f t="shared" si="26"/>
+        <v>106</v>
+      </c>
+      <c r="AC39" s="2">
+        <f t="shared" si="27"/>
+        <v>130</v>
+      </c>
+      <c r="AD39" s="2">
+        <f t="shared" si="28"/>
+        <v>130</v>
+      </c>
+      <c r="AE39" s="2">
+        <f t="shared" si="29"/>
+        <v>176</v>
+      </c>
+      <c r="AF39" s="2">
+        <f t="shared" si="30"/>
+        <v>170</v>
+      </c>
+      <c r="AG39" s="2">
+        <f t="shared" si="31"/>
+        <v>170</v>
+      </c>
+      <c r="AH39" s="2">
+        <f t="shared" si="32"/>
+        <v>170</v>
+      </c>
+      <c r="AI39" s="2">
+        <f t="shared" si="33"/>
+        <v>170</v>
+      </c>
+      <c r="AJ39" s="2">
+        <f t="shared" si="34"/>
+        <v>170</v>
+      </c>
+      <c r="AK39" s="2">
+        <f t="shared" si="35"/>
+        <v>220</v>
+      </c>
+      <c r="AL39" s="2">
+        <f t="shared" si="36"/>
+        <v>220</v>
+      </c>
+      <c r="AM39" s="2">
+        <f t="shared" si="37"/>
+        <v>250</v>
+      </c>
+      <c r="AN39" s="2">
+        <f t="shared" si="38"/>
+        <v>214</v>
+      </c>
+      <c r="AO39" s="7">
+        <f t="shared" si="39"/>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B40" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="C40" s="2">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="3"/>
+        <v>144</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="4"/>
+        <v>196</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" si="5"/>
+        <v>196</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="6"/>
+        <v>260</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="7"/>
+        <v>302</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="8"/>
+        <v>314</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="9"/>
+        <v>316</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="10"/>
+        <v>328</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="11"/>
+        <v>380</v>
+      </c>
+      <c r="M40" s="2">
+        <f t="shared" si="12"/>
+        <v>418</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="13"/>
+        <v>470</v>
+      </c>
+      <c r="O40" s="2">
+        <f t="shared" si="14"/>
+        <v>470</v>
+      </c>
+      <c r="P40" s="2">
+        <f t="shared" si="15"/>
+        <v>490</v>
+      </c>
+      <c r="Q40" s="2">
+        <f t="shared" si="16"/>
+        <v>528</v>
+      </c>
+      <c r="R40" s="2">
+        <f t="shared" si="17"/>
+        <v>528</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="18"/>
+        <v>528</v>
+      </c>
+      <c r="T40" s="7">
+        <f t="shared" si="19"/>
+        <v>528</v>
+      </c>
+      <c r="V40" s="6">
+        <f t="shared" si="20"/>
+        <v>54</v>
+      </c>
+      <c r="W40" s="2">
+        <f t="shared" si="21"/>
+        <v>58</v>
+      </c>
+      <c r="X40" s="2">
+        <f t="shared" si="22"/>
+        <v>80</v>
+      </c>
+      <c r="Y40" s="2">
+        <f t="shared" si="23"/>
+        <v>76</v>
+      </c>
+      <c r="Z40" s="2">
+        <f t="shared" si="24"/>
+        <v>102</v>
+      </c>
+      <c r="AA40" s="2">
+        <f t="shared" si="25"/>
+        <v>102</v>
+      </c>
+      <c r="AB40" s="2">
+        <f t="shared" si="26"/>
+        <v>142</v>
+      </c>
+      <c r="AC40" s="2">
+        <f t="shared" si="27"/>
+        <v>176</v>
+      </c>
+      <c r="AD40" s="2">
+        <f t="shared" si="28"/>
+        <v>188</v>
+      </c>
+      <c r="AE40" s="2">
+        <f t="shared" si="29"/>
+        <v>170</v>
+      </c>
+      <c r="AF40" s="2">
+        <f t="shared" si="30"/>
+        <v>170</v>
+      </c>
+      <c r="AG40" s="2">
+        <f t="shared" si="31"/>
+        <v>170</v>
+      </c>
+      <c r="AH40" s="2">
+        <f t="shared" si="32"/>
+        <v>170</v>
+      </c>
+      <c r="AI40" s="2">
+        <f t="shared" si="33"/>
+        <v>200</v>
+      </c>
+      <c r="AJ40" s="2">
+        <f t="shared" si="34"/>
+        <v>190</v>
+      </c>
+      <c r="AK40" s="2">
+        <f t="shared" si="35"/>
+        <v>210</v>
+      </c>
+      <c r="AL40" s="2">
+        <f t="shared" si="36"/>
+        <v>230</v>
+      </c>
+      <c r="AM40" s="2">
+        <f t="shared" si="37"/>
+        <v>214</v>
+      </c>
+      <c r="AN40" s="2">
+        <f t="shared" si="38"/>
+        <v>214</v>
+      </c>
+      <c r="AO40" s="7">
+        <f t="shared" si="39"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <f>A42+A19 * MOD(A19 + 1,2)</f>
+        <v>54</v>
+      </c>
+      <c r="B41" s="2">
+        <f>MAX(A41,B42) + B19 * MOD(B19 + 1,2)</f>
+        <v>54</v>
+      </c>
+      <c r="C41" s="2">
+        <f t="shared" ref="C41:T41" si="46">MAX(B41,C42) + C19 * MOD(C19 + 1,2)</f>
+        <v>122</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="46"/>
+        <v>130</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="46"/>
+        <v>170</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="46"/>
+        <v>170</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="46"/>
+        <v>220</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="46"/>
+        <v>268</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="46"/>
+        <v>302</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="46"/>
+        <v>302</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="46"/>
+        <v>328</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="46"/>
+        <v>380</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="46"/>
+        <v>418</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="46"/>
+        <v>440</v>
+      </c>
+      <c r="O41" s="2">
+        <f t="shared" si="46"/>
+        <v>440</v>
+      </c>
+      <c r="P41" s="2">
+        <f t="shared" si="46"/>
+        <v>440</v>
+      </c>
+      <c r="Q41" s="2">
+        <f t="shared" si="46"/>
+        <v>442</v>
+      </c>
+      <c r="R41" s="2">
+        <f t="shared" si="46"/>
+        <v>464</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="46"/>
+        <v>480</v>
+      </c>
+      <c r="T41" s="7">
+        <f t="shared" si="46"/>
+        <v>480</v>
+      </c>
+      <c r="V41" s="6">
+        <f>V42+A19 * MOD(A19 + 1,2)</f>
+        <v>54</v>
+      </c>
+      <c r="W41" s="2">
+        <f>MIN(V41,W42) + B19 * MOD(B19 + 1,2)</f>
+        <v>54</v>
+      </c>
+      <c r="X41" s="2">
+        <f t="shared" ref="X41:AO41" si="47">MIN(W41,X42) + C19 * MOD(C19 + 1,2)</f>
+        <v>108</v>
+      </c>
+      <c r="Y41" s="2">
+        <f t="shared" si="47"/>
+        <v>76</v>
+      </c>
+      <c r="Z41" s="2">
+        <f t="shared" si="47"/>
+        <v>116</v>
+      </c>
+      <c r="AA41" s="2">
+        <f t="shared" si="47"/>
+        <v>116</v>
+      </c>
+      <c r="AB41" s="2">
+        <f t="shared" si="47"/>
+        <v>166</v>
+      </c>
+      <c r="AC41" s="2">
+        <f t="shared" si="47"/>
+        <v>214</v>
+      </c>
+      <c r="AD41" s="2">
+        <f t="shared" si="47"/>
+        <v>202</v>
+      </c>
+      <c r="AE41" s="2">
+        <f t="shared" si="47"/>
+        <v>168</v>
+      </c>
+      <c r="AF41" s="2">
+        <f t="shared" si="47"/>
+        <v>194</v>
+      </c>
+      <c r="AG41" s="2">
+        <f t="shared" si="47"/>
+        <v>220</v>
+      </c>
+      <c r="AH41" s="2">
+        <f t="shared" si="47"/>
+        <v>206</v>
+      </c>
+      <c r="AI41" s="2">
+        <f t="shared" si="47"/>
+        <v>190</v>
+      </c>
+      <c r="AJ41" s="2">
+        <f t="shared" si="47"/>
+        <v>190</v>
+      </c>
+      <c r="AK41" s="2">
+        <f t="shared" si="47"/>
+        <v>190</v>
+      </c>
+      <c r="AL41" s="2">
+        <f t="shared" si="47"/>
+        <v>192</v>
+      </c>
+      <c r="AM41" s="2">
+        <f t="shared" si="47"/>
+        <v>214</v>
+      </c>
+      <c r="AN41" s="2">
+        <f t="shared" si="47"/>
+        <v>216</v>
+      </c>
+      <c r="AO41" s="7">
+        <f t="shared" si="47"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <f>A20</f>
+        <v>54</v>
+      </c>
+      <c r="B42" s="9">
+        <f>A42+B20 * MOD(B20 + 1, 2)</f>
+        <v>54</v>
+      </c>
+      <c r="C42" s="9">
+        <f t="shared" ref="C42:T42" si="48">B42+C20 * MOD(C20 + 1, 2)</f>
+        <v>68</v>
+      </c>
+      <c r="D42" s="9">
+        <f t="shared" si="48"/>
+        <v>68</v>
+      </c>
+      <c r="E42" s="9">
+        <f t="shared" si="48"/>
+        <v>122</v>
+      </c>
+      <c r="F42" s="9">
+        <f t="shared" si="48"/>
+        <v>122</v>
+      </c>
+      <c r="G42" s="9">
+        <f t="shared" si="48"/>
+        <v>122</v>
+      </c>
+      <c r="H42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="I42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="J42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="K42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="L42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="M42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="N42" s="9">
+        <f t="shared" si="48"/>
+        <v>168</v>
+      </c>
+      <c r="O42" s="9">
+        <f t="shared" si="48"/>
+        <v>190</v>
+      </c>
+      <c r="P42" s="9">
+        <f t="shared" si="48"/>
+        <v>190</v>
+      </c>
+      <c r="Q42" s="9">
+        <f t="shared" si="48"/>
+        <v>200</v>
+      </c>
+      <c r="R42" s="9">
+        <f t="shared" si="48"/>
+        <v>200</v>
+      </c>
+      <c r="S42" s="9">
+        <f t="shared" si="48"/>
+        <v>200</v>
+      </c>
+      <c r="T42" s="1">
+        <f t="shared" si="48"/>
+        <v>200</v>
+      </c>
+      <c r="V42" s="8">
+        <v>54</v>
+      </c>
+      <c r="W42" s="9">
+        <f>V42+B20 * MOD(B20 + 1, 2)</f>
+        <v>54</v>
+      </c>
+      <c r="X42" s="9">
+        <f t="shared" ref="X42:AO42" si="49">W42+C20 * MOD(C20 + 1, 2)</f>
+        <v>68</v>
+      </c>
+      <c r="Y42" s="9">
+        <f t="shared" si="49"/>
+        <v>68</v>
+      </c>
+      <c r="Z42" s="9">
+        <f t="shared" si="49"/>
+        <v>122</v>
+      </c>
+      <c r="AA42" s="9">
+        <f t="shared" si="49"/>
+        <v>122</v>
+      </c>
+      <c r="AB42" s="9">
+        <f t="shared" si="49"/>
+        <v>122</v>
+      </c>
+      <c r="AC42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AD42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AE42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AF42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AG42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AH42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AI42" s="9">
+        <f t="shared" si="49"/>
+        <v>168</v>
+      </c>
+      <c r="AJ42" s="9">
+        <f t="shared" si="49"/>
+        <v>190</v>
+      </c>
+      <c r="AK42" s="9">
+        <f t="shared" si="49"/>
+        <v>190</v>
+      </c>
+      <c r="AL42" s="9">
+        <f t="shared" si="49"/>
+        <v>200</v>
+      </c>
+      <c r="AM42" s="9">
+        <f t="shared" si="49"/>
+        <v>200</v>
+      </c>
+      <c r="AN42" s="9">
+        <f t="shared" si="49"/>
+        <v>200</v>
+      </c>
+      <c r="AO42" s="1">
+        <f t="shared" si="49"/>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>